<commit_message>
Create test data and build script test for signup page
</commit_message>
<xml_diff>
--- a/test-data/CreateAcount.xlsx
+++ b/test-data/CreateAcount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>FirstName</t>
   </si>
@@ -29,14 +29,85 @@
   </si>
   <si>
     <t>yoyo</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>PasswordConfirm</t>
+  </si>
+  <si>
+    <t>Birthday-Month</t>
+  </si>
+  <si>
+    <t>Birthday-Day</t>
+  </si>
+  <si>
+    <t>Birthday-Year</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>NameMesEr</t>
+  </si>
+  <si>
+    <t>UserNameMesEr</t>
+  </si>
+  <si>
+    <t>PasswordMesEr</t>
+  </si>
+  <si>
+    <t>PasswordConfirmMesEr</t>
+  </si>
+  <si>
+    <t>Birthday-MonthMesEr</t>
+  </si>
+  <si>
+    <t>Birthday-DayMesEr</t>
+  </si>
+  <si>
+    <t>Birthday-YearMesEr</t>
+  </si>
+  <si>
+    <t>GenderMesEr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>All field is blank</t>
+  </si>
+  <si>
+    <t>Only firstname and lastname are blank</t>
+  </si>
+  <si>
+    <t>Only firstname is blank</t>
+  </si>
+  <si>
+    <t>Only lastname is blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -52,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -60,12 +131,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,58 +458,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update data test and define elements for signup page
</commit_message>
<xml_diff>
--- a/test-data/CreateAcount.xlsx
+++ b/test-data/CreateAcount.xlsx
@@ -31,21 +31,6 @@
     <t>yoyo</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>PasswordConfirm</t>
-  </si>
-  <si>
-    <t>Birthday-Month</t>
-  </si>
-  <si>
-    <t>Birthday-Day</t>
-  </si>
-  <si>
-    <t>Birthday-Year</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -58,21 +43,6 @@
     <t>UserNameMesEr</t>
   </si>
   <si>
-    <t>PasswordMesEr</t>
-  </si>
-  <si>
-    <t>PasswordConfirmMesEr</t>
-  </si>
-  <si>
-    <t>Birthday-MonthMesEr</t>
-  </si>
-  <si>
-    <t>Birthday-DayMesEr</t>
-  </si>
-  <si>
-    <t>Birthday-YearMesEr</t>
-  </si>
-  <si>
     <t>GenderMesEr</t>
   </si>
   <si>
@@ -92,6 +62,36 @@
   </si>
   <si>
     <t>Only lastname is blank</t>
+  </si>
+  <si>
+    <t>BirthMonth</t>
+  </si>
+  <si>
+    <t>BirthDay</t>
+  </si>
+  <si>
+    <t>BirthYear</t>
+  </si>
+  <si>
+    <t>Passwd</t>
+  </si>
+  <si>
+    <t>PasswdConfirm</t>
+  </si>
+  <si>
+    <t>BirthMonthMesEr</t>
+  </si>
+  <si>
+    <t>BirthDayMesEr</t>
+  </si>
+  <si>
+    <t>BirthYearMesEr</t>
+  </si>
+  <si>
+    <t>PasswdMesEr</t>
+  </si>
+  <si>
+    <t>PasswdConfirmMesEr</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -500,60 +500,60 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -572,7 +572,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -582,7 +582,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -600,7 +600,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
create demo test with excel data
</commit_message>
<xml_diff>
--- a/test-data/CreateAcount.xlsx
+++ b/test-data/CreateAcount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>FirstName</t>
   </si>
@@ -25,12 +25,6 @@
     <t>UserName</t>
   </si>
   <si>
-    <t>Huy</t>
-  </si>
-  <si>
-    <t>yoyo</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -92,6 +86,18 @@
   </si>
   <si>
     <t>PasswdConfirmMesEr</t>
+  </si>
+  <si>
+    <t>ThoHip12345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> !@12345678</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -461,7 +467,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +494,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -500,60 +506,60 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -572,23 +578,35 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1">
         <v>13</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="1">
+        <v>1989</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -600,21 +618,35 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1989</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -626,17 +658,33 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1989</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>

</xml_diff>

<commit_message>
update test case demoExcelTestData - Input data from excel file
</commit_message>
<xml_diff>
--- a/test-data/CreateAcount.xlsx
+++ b/test-data/CreateAcount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>FirstName</t>
   </si>
@@ -40,9 +40,6 @@
     <t>GenderMesEr</t>
   </si>
   <si>
-    <t xml:space="preserve">   </t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -98,6 +95,24 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>CurrentEmail</t>
+  </si>
+  <si>
+    <t>dinhhuy131@gmail.com</t>
+  </si>
+  <si>
+    <t>0979155626</t>
+  </si>
+  <si>
+    <t>0979155627</t>
+  </si>
+  <si>
+    <t>0979155628</t>
   </si>
 </sst>
 </file>
@@ -156,10 +171,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,35 +480,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.75" customWidth="1"/>
+    <col min="2" max="2" width="10.125" customWidth="1"/>
+    <col min="3" max="3" width="9.75" customWidth="1"/>
+    <col min="4" max="4" width="10.375" customWidth="1"/>
+    <col min="5" max="5" width="9.375" customWidth="1"/>
+    <col min="6" max="6" width="16.75" customWidth="1"/>
+    <col min="7" max="7" width="15.25" customWidth="1"/>
+    <col min="8" max="8" width="12.375" customWidth="1"/>
+    <col min="9" max="9" width="13.25" customWidth="1"/>
+    <col min="10" max="10" width="7.75" customWidth="1"/>
+    <col min="11" max="11" width="12.25" customWidth="1"/>
+    <col min="12" max="12" width="20.875" customWidth="1"/>
+    <col min="13" max="13" width="11.875" customWidth="1"/>
+    <col min="14" max="14" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -506,60 +524,62 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -575,28 +595,26 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="H3" s="1">
         <v>13</v>
@@ -605,38 +623,42 @@
         <v>1989</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="H4" s="1">
         <v>13</v>
@@ -645,36 +667,42 @@
         <v>1989</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="H5" s="1">
         <v>13</v>
@@ -683,16 +711,22 @@
         <v>1989</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update demoExcelTestData - Add verify messages error
</commit_message>
<xml_diff>
--- a/test-data/CreateAcount.xlsx
+++ b/test-data/CreateAcount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>FirstName</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>NameMesEr</t>
-  </si>
-  <si>
     <t>UserNameMesEr</t>
   </si>
   <si>
@@ -113,6 +110,15 @@
   </si>
   <si>
     <t>0979155628</t>
+  </si>
+  <si>
+    <t>FirstNameMesEr</t>
+  </si>
+  <si>
+    <t>LastNameMesEr</t>
+  </si>
+  <si>
+    <t>You can't leave this empty.</t>
   </si>
 </sst>
 </file>
@@ -480,37 +486,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.75" customWidth="1"/>
-    <col min="2" max="2" width="10.125" customWidth="1"/>
-    <col min="3" max="3" width="9.75" customWidth="1"/>
-    <col min="4" max="4" width="10.375" customWidth="1"/>
-    <col min="5" max="5" width="9.375" customWidth="1"/>
-    <col min="6" max="6" width="16.75" customWidth="1"/>
-    <col min="7" max="7" width="15.25" customWidth="1"/>
-    <col min="8" max="8" width="12.375" customWidth="1"/>
-    <col min="9" max="9" width="13.25" customWidth="1"/>
-    <col min="10" max="10" width="7.75" customWidth="1"/>
-    <col min="11" max="11" width="12.25" customWidth="1"/>
-    <col min="12" max="12" width="20.875" customWidth="1"/>
-    <col min="13" max="13" width="11.875" customWidth="1"/>
-    <col min="14" max="14" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="24" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" customWidth="1"/>
+    <col min="14" max="14" width="25.7109375" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -524,62 +531,65 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -590,31 +600,36 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="N2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H3" s="1">
         <v>13</v>
@@ -623,42 +638,43 @@
         <v>1989</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H4" s="1">
         <v>13</v>
@@ -667,42 +683,47 @@
         <v>1989</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H5" s="1">
         <v>13</v>
@@ -711,22 +732,25 @@
         <v>1989</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>